<commit_message>
adds nutrition bits (req adds for logical connections between vars)
</commit_message>
<xml_diff>
--- a/inst/extdata/MSF-survey-dict.xlsx
+++ b/inst/extdata/MSF-survey-dict.xlsx
@@ -575,9 +575,6 @@
     <t>oedema</t>
   </si>
   <si>
-    <t>age_months</t>
-  </si>
-  <si>
     <t>sex</t>
   </si>
   <si>
@@ -966,6 +963,9 @@
   </si>
   <si>
     <t>q77_what_is_the_cluster_number</t>
+  </si>
+  <si>
+    <t>age_month</t>
   </si>
 </sst>
 </file>
@@ -3424,7 +3424,7 @@
   <dimension ref="A1:F27"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="P17" sqref="P17"/>
+      <selection activeCell="O15" sqref="O15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3459,10 +3459,10 @@
         <v>0</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="D2" s="2" t="s">
         <v>0</v>
@@ -3477,10 +3477,10 @@
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="4"/>
       <c r="B3" s="2" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="D3" s="2" t="s">
         <v>0</v>
@@ -3495,10 +3495,10 @@
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="4"/>
       <c r="B4" s="2" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="D4" s="2" t="s">
         <v>3</v>
@@ -3513,10 +3513,10 @@
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="4"/>
       <c r="B5" s="2" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="D5" s="2" t="s">
         <v>3</v>
@@ -3707,7 +3707,7 @@
         <v>1</v>
       </c>
       <c r="B17" s="4" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="C17" s="4" t="s">
         <v>122</v>
@@ -3739,7 +3739,7 @@
     <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19" s="4"/>
       <c r="B19" s="2" t="s">
-        <v>184</v>
+        <v>314</v>
       </c>
       <c r="C19" s="2" t="s">
         <v>119</v>
@@ -3946,10 +3946,10 @@
         <v>0</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="D2" s="2" t="s">
         <v>0</v>
@@ -3964,10 +3964,10 @@
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="4"/>
       <c r="B3" s="2" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="D3" s="2" t="s">
         <v>0</v>
@@ -3982,16 +3982,16 @@
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="4"/>
       <c r="B4" s="4" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="D4" s="2" t="s">
         <v>4</v>
       </c>
       <c r="E4" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="F4" t="s">
         <v>173</v>
@@ -4005,7 +4005,7 @@
         <v>43</v>
       </c>
       <c r="E5" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="F5" t="s">
         <v>173</v>
@@ -4019,7 +4019,7 @@
         <v>46</v>
       </c>
       <c r="E6" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="F6" t="s">
         <v>173</v>
@@ -4033,7 +4033,7 @@
         <v>47</v>
       </c>
       <c r="E7" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="F7" t="s">
         <v>173</v>
@@ -4047,7 +4047,7 @@
         <v>44</v>
       </c>
       <c r="E8" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="F8" t="s">
         <v>173</v>
@@ -4058,7 +4058,7 @@
       <c r="B9" s="4"/>
       <c r="C9" s="4"/>
       <c r="D9" s="2" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="E9" t="s">
         <v>16</v>
@@ -4070,10 +4070,10 @@
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" s="4"/>
       <c r="B10" s="2" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="D10" s="2" t="s">
         <v>0</v>
@@ -4088,10 +4088,10 @@
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" s="4"/>
       <c r="B11" s="4" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="C11" s="4" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="D11" s="2" t="s">
         <v>4</v>
@@ -4120,10 +4120,10 @@
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" s="4"/>
       <c r="B13" s="2" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="D13" s="2" t="s">
         <v>0</v>
@@ -4138,10 +4138,10 @@
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" s="4"/>
       <c r="B14" s="4" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="C14" s="4" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="D14" s="2" t="s">
         <v>4</v>
@@ -4170,16 +4170,16 @@
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" s="4"/>
       <c r="B16" s="4" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="C16" s="4" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="D16" s="2" t="s">
         <v>43</v>
       </c>
       <c r="E16" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="F16" t="s">
         <v>173</v>
@@ -4193,7 +4193,7 @@
         <v>46</v>
       </c>
       <c r="E17" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="F17" t="s">
         <v>173</v>
@@ -4207,7 +4207,7 @@
         <v>46</v>
       </c>
       <c r="E18" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="F18" t="s">
         <v>173</v>
@@ -4221,7 +4221,7 @@
         <v>47</v>
       </c>
       <c r="E19" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="F19" t="s">
         <v>173</v>
@@ -4235,7 +4235,7 @@
         <v>44</v>
       </c>
       <c r="E20" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="F20" t="s">
         <v>173</v>
@@ -4249,7 +4249,7 @@
         <v>45</v>
       </c>
       <c r="E21" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="F21" t="s">
         <v>173</v>
@@ -4263,7 +4263,7 @@
         <v>48</v>
       </c>
       <c r="E22" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="F22" t="s">
         <v>173</v>
@@ -4277,7 +4277,7 @@
         <v>49</v>
       </c>
       <c r="E23" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="F23" t="s">
         <v>173</v>
@@ -4300,10 +4300,10 @@
     <row r="25" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A25" s="4"/>
       <c r="B25" s="2" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="C25" s="2" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="D25" s="2" t="s">
         <v>0</v>
@@ -4318,10 +4318,10 @@
     <row r="26" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A26" s="4"/>
       <c r="B26" s="4" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="C26" s="4" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="D26" s="2" t="s">
         <v>4</v>
@@ -4341,7 +4341,7 @@
         <v>43</v>
       </c>
       <c r="E27" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="F27" t="s">
         <v>173</v>
@@ -4369,7 +4369,7 @@
         <v>47</v>
       </c>
       <c r="E29" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="F29" t="s">
         <v>173</v>
@@ -4378,10 +4378,10 @@
     <row r="30" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A30" s="4"/>
       <c r="B30" s="2" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="C30" s="2" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="D30" s="2" t="s">
         <v>0</v>
@@ -4398,10 +4398,10 @@
         <v>1</v>
       </c>
       <c r="B31" s="4" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="C31" s="4" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="D31" s="2" t="s">
         <v>4</v>
@@ -4430,10 +4430,10 @@
     <row r="33" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A33" s="4"/>
       <c r="B33" s="2" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="C33" s="2" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="D33" s="2" t="s">
         <v>0</v>
@@ -4448,10 +4448,10 @@
     <row r="34" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A34" s="4"/>
       <c r="B34" s="2" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="C34" s="2" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="D34" s="2" t="s">
         <v>0</v>
@@ -4466,10 +4466,10 @@
     <row r="35" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A35" s="4"/>
       <c r="B35" s="4" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="C35" s="4" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="D35" s="2" t="s">
         <v>3</v>
@@ -4489,7 +4489,7 @@
         <v>4</v>
       </c>
       <c r="E36" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="F36" t="s">
         <v>173</v>
@@ -4503,7 +4503,7 @@
         <v>43</v>
       </c>
       <c r="E37" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="F37" t="s">
         <v>173</v>
@@ -4517,7 +4517,7 @@
         <v>46</v>
       </c>
       <c r="E38" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="F38" t="s">
         <v>173</v>
@@ -4531,7 +4531,7 @@
         <v>17</v>
       </c>
       <c r="E39" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="F39" t="s">
         <v>173</v>
@@ -4540,10 +4540,10 @@
     <row r="40" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A40" s="4"/>
       <c r="B40" s="2" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="C40" s="2" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="D40" s="2" t="s">
         <v>0</v>
@@ -4558,10 +4558,10 @@
     <row r="41" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A41" s="4"/>
       <c r="B41" s="2" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="C41" s="2" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="D41" s="2" t="s">
         <v>0</v>
@@ -4576,16 +4576,16 @@
     <row r="42" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A42" s="4"/>
       <c r="B42" s="4" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="C42" s="4" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="D42" s="2" t="s">
         <v>4</v>
       </c>
       <c r="E42" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="F42" t="s">
         <v>173</v>
@@ -4599,7 +4599,7 @@
         <v>43</v>
       </c>
       <c r="E43" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="F43" t="s">
         <v>173</v>
@@ -4613,7 +4613,7 @@
         <v>46</v>
       </c>
       <c r="E44" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="F44" t="s">
         <v>173</v>
@@ -4624,7 +4624,7 @@
       <c r="B45" s="4"/>
       <c r="C45" s="4"/>
       <c r="D45" s="2" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="E45" t="s">
         <v>16</v>
@@ -4636,10 +4636,10 @@
     <row r="46" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A46" s="4"/>
       <c r="B46" s="2" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="C46" s="2" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="D46" s="2" t="s">
         <v>0</v>
@@ -4654,16 +4654,16 @@
     <row r="47" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A47" s="4"/>
       <c r="B47" s="4" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="C47" s="4" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="D47" s="2" t="s">
         <v>4</v>
       </c>
       <c r="E47" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="F47" t="s">
         <v>173</v>
@@ -4677,7 +4677,7 @@
         <v>43</v>
       </c>
       <c r="E48" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="F48" t="s">
         <v>173</v>
@@ -4691,7 +4691,7 @@
         <v>46</v>
       </c>
       <c r="E49" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="F49" t="s">
         <v>173</v>
@@ -4705,7 +4705,7 @@
         <v>47</v>
       </c>
       <c r="E50" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="F50" t="s">
         <v>173</v>
@@ -4719,7 +4719,7 @@
         <v>44</v>
       </c>
       <c r="E51" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="F51" t="s">
         <v>173</v>
@@ -4733,7 +4733,7 @@
         <v>45</v>
       </c>
       <c r="E52" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="F52" t="s">
         <v>173</v>
@@ -4747,7 +4747,7 @@
         <v>48</v>
       </c>
       <c r="E53" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="F53" t="s">
         <v>173</v>
@@ -4761,7 +4761,7 @@
         <v>49</v>
       </c>
       <c r="E54" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="F54" t="s">
         <v>173</v>
@@ -4775,7 +4775,7 @@
         <v>17</v>
       </c>
       <c r="E55" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="F55" t="s">
         <v>173</v>
@@ -4789,7 +4789,7 @@
         <v>50</v>
       </c>
       <c r="E56" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="F56" t="s">
         <v>173</v>
@@ -4798,10 +4798,10 @@
     <row r="57" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A57" s="4"/>
       <c r="B57" s="2" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="C57" s="2" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="D57" s="2" t="s">
         <v>0</v>
@@ -4816,10 +4816,10 @@
     <row r="58" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A58" s="4"/>
       <c r="B58" s="4" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="C58" s="4" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="D58" s="2" t="s">
         <v>3</v>
@@ -4839,7 +4839,7 @@
         <v>4</v>
       </c>
       <c r="E59" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="F59" t="s">
         <v>173</v>
@@ -4853,7 +4853,7 @@
         <v>43</v>
       </c>
       <c r="E60" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="F60" t="s">
         <v>173</v>
@@ -4867,7 +4867,7 @@
         <v>46</v>
       </c>
       <c r="E61" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="F61" t="s">
         <v>173</v>
@@ -4881,7 +4881,7 @@
         <v>17</v>
       </c>
       <c r="E62" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="F62" t="s">
         <v>173</v>
@@ -4890,16 +4890,16 @@
     <row r="63" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A63" s="4"/>
       <c r="B63" s="4" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="C63" s="4" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="D63" s="2" t="s">
         <v>4</v>
       </c>
       <c r="E63" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="F63" t="s">
         <v>173</v>
@@ -4913,7 +4913,7 @@
         <v>43</v>
       </c>
       <c r="E64" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="F64" t="s">
         <v>173</v>
@@ -4927,7 +4927,7 @@
         <v>46</v>
       </c>
       <c r="E65" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="F65" t="s">
         <v>173</v>
@@ -4941,7 +4941,7 @@
         <v>47</v>
       </c>
       <c r="E66" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="F66" t="s">
         <v>173</v>
@@ -4955,7 +4955,7 @@
         <v>44</v>
       </c>
       <c r="E67" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="F67" t="s">
         <v>173</v>
@@ -4969,7 +4969,7 @@
         <v>45</v>
       </c>
       <c r="E68" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="F68" t="s">
         <v>173</v>
@@ -4983,7 +4983,7 @@
         <v>48</v>
       </c>
       <c r="E69" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="F69" t="s">
         <v>173</v>
@@ -4997,7 +4997,7 @@
         <v>49</v>
       </c>
       <c r="E70" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="F70" t="s">
         <v>173</v>
@@ -5011,7 +5011,7 @@
         <v>17</v>
       </c>
       <c r="E71" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="F71" t="s">
         <v>173</v>
@@ -5025,7 +5025,7 @@
         <v>50</v>
       </c>
       <c r="E72" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="F72" t="s">
         <v>173</v>
@@ -5034,10 +5034,10 @@
     <row r="73" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A73" s="4"/>
       <c r="B73" s="2" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="C73" s="2" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="D73" s="2" t="s">
         <v>0</v>
@@ -5052,10 +5052,10 @@
     <row r="74" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A74" s="4"/>
       <c r="B74" s="2" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="C74" s="2" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="D74" s="2" t="s">
         <v>0</v>
@@ -5070,10 +5070,10 @@
     <row r="75" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A75" s="4"/>
       <c r="B75" s="2" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="C75" s="2" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="D75" s="2" t="s">
         <v>0</v>
@@ -5088,16 +5088,16 @@
     <row r="76" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A76" s="4"/>
       <c r="B76" s="4" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="C76" s="4" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="D76" s="2" t="s">
         <v>4</v>
       </c>
       <c r="E76" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="F76" t="s">
         <v>173</v>
@@ -5111,7 +5111,7 @@
         <v>43</v>
       </c>
       <c r="E77" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="F77" t="s">
         <v>173</v>
@@ -5125,7 +5125,7 @@
         <v>46</v>
       </c>
       <c r="E78" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="F78" t="s">
         <v>173</v>
@@ -5136,7 +5136,7 @@
       <c r="B79" s="4"/>
       <c r="C79" s="4"/>
       <c r="D79" s="2" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="E79" t="s">
         <v>16</v>
@@ -5148,10 +5148,10 @@
     <row r="80" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A80" s="4"/>
       <c r="B80" s="2" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="C80" s="2" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="D80" s="2" t="s">
         <v>0</v>
@@ -5166,10 +5166,10 @@
     <row r="81" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A81" s="4"/>
       <c r="B81" s="4" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="C81" s="4" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="D81" s="2" t="s">
         <v>3</v>
@@ -5189,7 +5189,7 @@
         <v>4</v>
       </c>
       <c r="E82" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="F82" t="s">
         <v>173</v>
@@ -5203,7 +5203,7 @@
         <v>43</v>
       </c>
       <c r="E83" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="F83" t="s">
         <v>173</v>
@@ -5217,7 +5217,7 @@
         <v>46</v>
       </c>
       <c r="E84" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="F84" t="s">
         <v>173</v>
@@ -5231,7 +5231,7 @@
         <v>47</v>
       </c>
       <c r="E85" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="F85" t="s">
         <v>173</v>
@@ -5240,10 +5240,10 @@
     <row r="86" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A86" s="4"/>
       <c r="B86" s="2" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="C86" s="2" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="D86" s="2" t="s">
         <v>0</v>
@@ -5258,10 +5258,10 @@
     <row r="87" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A87" s="4"/>
       <c r="B87" s="2" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="C87" s="2" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="D87" s="2" t="s">
         <v>0</v>
@@ -5276,16 +5276,16 @@
     <row r="88" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A88" s="4"/>
       <c r="B88" s="4" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="C88" s="4" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="D88" s="2" t="s">
         <v>4</v>
       </c>
       <c r="E88" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="F88" t="s">
         <v>173</v>
@@ -5299,7 +5299,7 @@
         <v>43</v>
       </c>
       <c r="E89" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="F89" t="s">
         <v>173</v>
@@ -5313,7 +5313,7 @@
         <v>46</v>
       </c>
       <c r="E90" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="F90" t="s">
         <v>173</v>
@@ -5324,7 +5324,7 @@
       <c r="B91" s="4"/>
       <c r="C91" s="4"/>
       <c r="D91" s="2" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="E91" t="s">
         <v>16</v>
@@ -5336,10 +5336,10 @@
     <row r="92" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A92" s="4"/>
       <c r="B92" s="2" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="C92" s="2" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="D92" s="2" t="s">
         <v>0</v>
@@ -5354,16 +5354,16 @@
     <row r="93" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A93" s="4"/>
       <c r="B93" s="4" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="C93" s="4" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="D93" s="2" t="s">
         <v>4</v>
       </c>
       <c r="E93" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="F93" t="s">
         <v>173</v>
@@ -5377,7 +5377,7 @@
         <v>43</v>
       </c>
       <c r="E94" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="F94" t="s">
         <v>173</v>
@@ -5391,7 +5391,7 @@
         <v>46</v>
       </c>
       <c r="E95" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="F95" t="s">
         <v>173</v>
@@ -5405,7 +5405,7 @@
         <v>47</v>
       </c>
       <c r="E96" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="F96" t="s">
         <v>173</v>
@@ -5419,7 +5419,7 @@
         <v>44</v>
       </c>
       <c r="E97" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="F97" t="s">
         <v>173</v>
@@ -5433,7 +5433,7 @@
         <v>45</v>
       </c>
       <c r="E98" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="F98" t="s">
         <v>173</v>
@@ -5447,7 +5447,7 @@
         <v>48</v>
       </c>
       <c r="E99" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="F99" t="s">
         <v>173</v>
@@ -5461,7 +5461,7 @@
         <v>49</v>
       </c>
       <c r="E100" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="F100" t="s">
         <v>173</v>
@@ -5475,7 +5475,7 @@
         <v>17</v>
       </c>
       <c r="E101" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="F101" t="s">
         <v>173</v>
@@ -5489,7 +5489,7 @@
         <v>50</v>
       </c>
       <c r="E102" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="F102" t="s">
         <v>173</v>
@@ -5500,10 +5500,10 @@
       <c r="B103" s="4"/>
       <c r="C103" s="4"/>
       <c r="D103" s="2" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="E103" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="F103" t="s">
         <v>173</v>
@@ -5514,10 +5514,10 @@
       <c r="B104" s="4"/>
       <c r="C104" s="4"/>
       <c r="D104" s="2" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="E104" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="F104" t="s">
         <v>173</v>
@@ -5528,10 +5528,10 @@
       <c r="B105" s="4"/>
       <c r="C105" s="4"/>
       <c r="D105" s="2" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="E105" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="F105" t="s">
         <v>173</v>
@@ -5542,10 +5542,10 @@
       <c r="B106" s="4"/>
       <c r="C106" s="4"/>
       <c r="D106" s="2" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="E106" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="F106" t="s">
         <v>173</v>
@@ -5556,10 +5556,10 @@
       <c r="B107" s="4"/>
       <c r="C107" s="4"/>
       <c r="D107" s="2" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="E107" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="F107" t="s">
         <v>173</v>
@@ -5570,10 +5570,10 @@
       <c r="B108" s="4"/>
       <c r="C108" s="4"/>
       <c r="D108" s="2" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="E108" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="F108" t="s">
         <v>173</v>
@@ -5584,10 +5584,10 @@
       <c r="B109" s="4"/>
       <c r="C109" s="4"/>
       <c r="D109" s="2" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="E109" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="F109" t="s">
         <v>173</v>
@@ -5598,10 +5598,10 @@
       <c r="B110" s="4"/>
       <c r="C110" s="4"/>
       <c r="D110" s="2" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="E110" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="F110" t="s">
         <v>173</v>
@@ -5612,10 +5612,10 @@
       <c r="B111" s="4"/>
       <c r="C111" s="4"/>
       <c r="D111" s="2" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="E111" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="F111" t="s">
         <v>173</v>
@@ -5624,10 +5624,10 @@
     <row r="112" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A112" s="4"/>
       <c r="B112" s="2" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="C112" s="2" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="D112" s="2" t="s">
         <v>0</v>
@@ -5642,10 +5642,10 @@
     <row r="113" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A113" s="4"/>
       <c r="B113" s="4" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="C113" s="4" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="D113" s="2" t="s">
         <v>4</v>
@@ -5679,7 +5679,7 @@
         <v>43</v>
       </c>
       <c r="E115" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="F115" t="s">
         <v>173</v>
@@ -5688,10 +5688,10 @@
     <row r="116" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A116" s="4"/>
       <c r="B116" s="2" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="C116" s="2" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="D116" s="2" t="s">
         <v>0</v>
@@ -5706,10 +5706,10 @@
     <row r="117" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A117" s="4"/>
       <c r="B117" s="2" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="C117" s="2" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="D117" s="2" t="s">
         <v>0</v>
@@ -5723,8 +5723,6 @@
     </row>
   </sheetData>
   <mergeCells count="34">
-    <mergeCell ref="B42:B45"/>
-    <mergeCell ref="B47:B56"/>
     <mergeCell ref="B113:B115"/>
     <mergeCell ref="A2:A30"/>
     <mergeCell ref="A31:A117"/>
@@ -5749,6 +5747,8 @@
     <mergeCell ref="C16:C24"/>
     <mergeCell ref="C81:C85"/>
     <mergeCell ref="C26:C29"/>
+    <mergeCell ref="B42:B45"/>
+    <mergeCell ref="B47:B56"/>
     <mergeCell ref="C113:C115"/>
     <mergeCell ref="C58:C62"/>
     <mergeCell ref="C63:C72"/>

</xml_diff>